<commit_message>
Add centrality and position to regression
</commit_message>
<xml_diff>
--- a/report/Book1-Synchronocity.xlsx
+++ b/report/Book1-Synchronocity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Finance(Prof.Heidari-Aghajanzadeh)\Project\Price-Synchronocity\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2761FB0-2631-4F01-8BB8-D2AE668EB49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA99C15-AF49-4A6F-9E36-A8C6C9A188E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{605FB5A5-1C5E-4F3D-AA02-B2E13B80D59B}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="23040" windowHeight="11724" xr2:uid="{605FB5A5-1C5E-4F3D-AA02-B2E13B80D59B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>mean</t>
   </si>
@@ -58,6 +58,30 @@
   </si>
   <si>
     <t>SYNCH</t>
+  </si>
+  <si>
+    <t>rsquared</t>
+  </si>
+  <si>
+    <t>position</t>
+  </si>
+  <si>
+    <t>Excess</t>
+  </si>
+  <si>
+    <t>leverage</t>
+  </si>
+  <si>
+    <t>centrality</t>
+  </si>
+  <si>
+    <t>ExcessDiff</t>
+  </si>
+  <si>
+    <t>ExcessDummy</t>
+  </si>
+  <si>
+    <t>ExcessHigh</t>
   </si>
 </sst>
 </file>
@@ -93,11 +117,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,20 +438,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B650B5-470C-415F-ADE6-AAC142A7394B}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="C2:K21"/>
+  <dimension ref="C2:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:J7"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="Q16" sqref="D16:Q16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:17" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>0</v>
       </c>
@@ -449,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>4</v>
       </c>
@@ -475,7 +502,7 @@
         <v>0.99999899999999997</v>
       </c>
     </row>
-    <row r="4" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C4" t="s">
         <v>5</v>
       </c>
@@ -501,7 +528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -527,7 +554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>7</v>
       </c>
@@ -553,7 +580,7 @@
         <v>45.569560000000003</v>
       </c>
     </row>
-    <row r="7" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>8</v>
       </c>
@@ -579,7 +606,7 @@
         <v>-12.517785</v>
       </c>
     </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>9</v>
       </c>
@@ -605,7 +632,7 @@
         <v>34.227831000000002</v>
       </c>
     </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>10</v>
       </c>
@@ -631,15 +658,10 @@
         <v>13.84689</v>
       </c>
     </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.3">
-      <c r="E14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="3">
-        <v>1127</v>
-      </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="3:17" x14ac:dyDescent="0.3">
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
@@ -647,45 +669,525 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="17" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-    </row>
-    <row r="18" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-    </row>
-    <row r="20" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-    </row>
-    <row r="21" spans="6:11" x14ac:dyDescent="0.3">
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
+    <row r="16" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2</v>
+      </c>
+      <c r="F16" s="4">
+        <v>3</v>
+      </c>
+      <c r="G16" s="4">
+        <v>4</v>
+      </c>
+      <c r="H16" s="4">
+        <v>5</v>
+      </c>
+      <c r="I16" s="4">
+        <v>6</v>
+      </c>
+      <c r="J16" s="4">
+        <v>7</v>
+      </c>
+      <c r="K16" s="4">
+        <v>8</v>
+      </c>
+      <c r="L16" s="4">
+        <v>9</v>
+      </c>
+      <c r="M16" s="4">
+        <v>10</v>
+      </c>
+      <c r="N16" s="4">
+        <v>11</v>
+      </c>
+      <c r="O16" s="4">
+        <v>12</v>
+      </c>
+      <c r="P16" s="4">
+        <v>13</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0.89829999999999999</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3">
+        <v>-7.1999999999999998E-3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>-3.4000000000000002E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>1</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3">
+        <v>-0.13159999999999999</v>
+      </c>
+      <c r="E20" s="3">
+        <v>-0.12790000000000001</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.47049999999999997</v>
+      </c>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" s="3">
+        <v>-6.7299999999999999E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>-5.1799999999999999E-2</v>
+      </c>
+      <c r="F21" s="3">
+        <v>-0.4849</v>
+      </c>
+      <c r="G21" s="3">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3">
+        <v>-1.34E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>-7.4999999999999997E-3</v>
+      </c>
+      <c r="F22" s="3">
+        <v>-3.2199999999999999E-2</v>
+      </c>
+      <c r="G22" s="3">
+        <v>-5.1499999999999997E-2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>1.9E-2</v>
+      </c>
+      <c r="I22" s="3">
+        <v>1</v>
+      </c>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+    </row>
+    <row r="23" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="3">
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="F23" s="3">
+        <v>6.7699999999999996E-2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>-0.17710000000000001</v>
+      </c>
+      <c r="H23" s="3">
+        <v>-0.1353</v>
+      </c>
+      <c r="I23" s="3">
+        <v>-1.9699999999999999E-2</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="3">
+        <v>-0.23089999999999999</v>
+      </c>
+      <c r="E24" s="3">
+        <v>-0.2351</v>
+      </c>
+      <c r="F24" s="3">
+        <v>-2.6800000000000001E-2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>0.14119999999999999</v>
+      </c>
+      <c r="H24" s="3">
+        <v>0.13589999999999999</v>
+      </c>
+      <c r="I24" s="3">
+        <v>0.1593</v>
+      </c>
+      <c r="J24" s="3">
+        <v>-0.2382</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3">
+        <v>7.7100000000000002E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="F25" s="3">
+        <v>0.19470000000000001</v>
+      </c>
+      <c r="G25" s="3">
+        <v>-8.5199999999999998E-2</v>
+      </c>
+      <c r="H25" s="3">
+        <v>-0.27260000000000001</v>
+      </c>
+      <c r="I25" s="3">
+        <v>-0.1103</v>
+      </c>
+      <c r="J25" s="3">
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="K25" s="3">
+        <v>-0.68740000000000001</v>
+      </c>
+      <c r="L25" s="3">
+        <v>1</v>
+      </c>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D26" s="3">
+        <v>-7.5200000000000003E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>-3.6299999999999999E-2</v>
+      </c>
+      <c r="F26" s="3">
+        <v>-0.8125</v>
+      </c>
+      <c r="G26" s="3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>0.64090000000000003</v>
+      </c>
+      <c r="I26" s="3">
+        <v>-1E-3</v>
+      </c>
+      <c r="J26" s="3">
+        <v>-0.20699999999999999</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0.12230000000000001</v>
+      </c>
+      <c r="L26" s="3">
+        <v>-0.30149999999999999</v>
+      </c>
+      <c r="M26" s="3">
+        <v>1</v>
+      </c>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="3">
+        <v>-0.1023</v>
+      </c>
+      <c r="E27" s="3">
+        <v>-7.0499999999999993E-2</v>
+      </c>
+      <c r="F27" s="3">
+        <v>-0.67530000000000001</v>
+      </c>
+      <c r="G27" s="3">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="H27" s="3">
+        <v>0.59430000000000005</v>
+      </c>
+      <c r="I27" s="3">
+        <v>-8.6E-3</v>
+      </c>
+      <c r="J27" s="3">
+        <v>-0.22040000000000001</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="L27" s="3">
+        <v>-0.27929999999999999</v>
+      </c>
+      <c r="M27" s="3">
+        <v>0.93269999999999997</v>
+      </c>
+      <c r="N27" s="3">
+        <v>1</v>
+      </c>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="3">
+        <v>-9.7199999999999995E-2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>-6.2899999999999998E-2</v>
+      </c>
+      <c r="F28" s="3">
+        <v>-0.55259999999999998</v>
+      </c>
+      <c r="G28" s="3">
+        <v>0.1108</v>
+      </c>
+      <c r="H28" s="3">
+        <v>0.4647</v>
+      </c>
+      <c r="I28" s="3">
+        <v>2.4199999999999999E-2</v>
+      </c>
+      <c r="J28" s="3">
+        <v>-0.1434</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0.1852</v>
+      </c>
+      <c r="L28" s="3">
+        <v>-0.25209999999999999</v>
+      </c>
+      <c r="M28" s="3">
+        <v>0.72230000000000005</v>
+      </c>
+      <c r="N28" s="3">
+        <v>0.68320000000000003</v>
+      </c>
+      <c r="O28" s="3">
+        <v>1</v>
+      </c>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="3">
+        <v>-9.0999999999999998E-2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>-6.5600000000000006E-2</v>
+      </c>
+      <c r="F29" s="3">
+        <v>-0.69440000000000002</v>
+      </c>
+      <c r="G29" s="3">
+        <v>0.1019</v>
+      </c>
+      <c r="H29" s="3">
+        <v>0.55089999999999995</v>
+      </c>
+      <c r="I29" s="3">
+        <v>-3.1800000000000002E-2</v>
+      </c>
+      <c r="J29" s="3">
+        <v>-0.1883</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0.14430000000000001</v>
+      </c>
+      <c r="L29" s="3">
+        <v>-0.27060000000000001</v>
+      </c>
+      <c r="M29" s="3">
+        <v>0.87429999999999997</v>
+      </c>
+      <c r="N29" s="3">
+        <v>0.82730000000000004</v>
+      </c>
+      <c r="O29" s="3">
+        <v>0.71020000000000005</v>
+      </c>
+      <c r="P29" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q29" s="3"/>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3">
+        <v>-0.1067</v>
+      </c>
+      <c r="E30" s="3">
+        <v>-7.3899999999999993E-2</v>
+      </c>
+      <c r="F30" s="3">
+        <v>-9.6600000000000005E-2</v>
+      </c>
+      <c r="G30" s="3">
+        <v>-4.6300000000000001E-2</v>
+      </c>
+      <c r="H30" s="3">
+        <v>-6.0400000000000002E-2</v>
+      </c>
+      <c r="I30" s="3">
+        <v>-5.0299999999999997E-2</v>
+      </c>
+      <c r="J30" s="3">
+        <v>-0.23169999999999999</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0.1032</v>
+      </c>
+      <c r="L30" s="3">
+        <v>-0.16919999999999999</v>
+      </c>
+      <c r="M30" s="3">
+        <v>0.104</v>
+      </c>
+      <c r="N30" s="3">
+        <v>6.4600000000000005E-2</v>
+      </c>
+      <c r="O30" s="3">
+        <v>4.9799999999999997E-2</v>
+      </c>
+      <c r="P30" s="3">
+        <v>0.1143</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>